<commit_message>
Add support for STM32L151xBA and IMST282A in mbed-os
</commit_message>
<xml_diff>
--- a/Calibration/Calibration_spreadsheet.xlsx
+++ b/Calibration/Calibration_spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pestourb\Documents\GitHub\Poucet_LCIS_LoRa24\Calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0AC8F50-BFA1-4C49-858A-7C4A869344EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4541A6F0-8340-40CD-A607-278E4E736CE7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6555" xr2:uid="{1BF5BE83-AB8A-4885-9800-215DE8CF36D3}"/>
   </bookViews>
@@ -463,8 +463,8 @@
   </sheetPr>
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>